<commit_message>
Adds Monaco csv files and clones app.py for Monaco specific plots.
</commit_message>
<xml_diff>
--- a/Laptime CSV Data/2023 Season/MonacoGP/2023 Monaco Quali.xlsx
+++ b/Laptime CSV Data/2023 Season/MonacoGP/2023 Monaco Quali.xlsx
@@ -1,25 +1,263 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\webstert\Side_Projects\Race-Strategy-Analysis\Laptime CSV Data\2023 Season\MonacoGP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D60C300-3E21-40CC-A942-775A51A563BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>EO</t>
+  </si>
+  <si>
+    <t>1 14 Fernando ALONSO 18.496</t>
+  </si>
+  <si>
+    <t>2 1 Max VERSTAPPEN 18.642</t>
+  </si>
+  <si>
+    <t>3 16 Charles LECLERC 18.651</t>
+  </si>
+  <si>
+    <t>14 Fernando ALONSO 33.844</t>
+  </si>
+  <si>
+    <t>55 Carlos SAINZ 33.856</t>
+  </si>
+  <si>
+    <t>16 Charles LECLERC 33.870</t>
+  </si>
+  <si>
+    <t>1 Max VERSTAPPEN 33.902</t>
+  </si>
+  <si>
+    <t>31 Esteban OCON 33.903</t>
+  </si>
+  <si>
+    <t>4 63 George RUSSELL 18.665</t>
+  </si>
+  <si>
+    <t>5 31 Esteban OCON 18.728</t>
+  </si>
+  <si>
+    <t>6 22 Yuki TSUNODA 18.746</t>
+  </si>
+  <si>
+    <t>7 44 Lewis HAMILTON 18.757</t>
+  </si>
+  <si>
+    <t>8 55 Carlos SAINZ 18.774</t>
+  </si>
+  <si>
+    <t>9 4 Lando NORRIS 18.807</t>
+  </si>
+  <si>
+    <t>10 81 Oscar PIASTRI 18.839</t>
+  </si>
+  <si>
+    <t>11 10 Pierre GASLY 18.841</t>
+  </si>
+  <si>
+    <t>12 18 Lance STROLL 18.853</t>
+  </si>
+  <si>
+    <t>13 21 Nyck DE VRIES 18.900</t>
+  </si>
+  <si>
+    <t>14 77 Valtteri BOTTAS 18.914</t>
+  </si>
+  <si>
+    <t>15 23 Alexander ALBON 18.989</t>
+  </si>
+  <si>
+    <t>16 24 ZHOU Guanyu 19.070</t>
+  </si>
+  <si>
+    <t>17 2 Logan SARGEANT 19.073</t>
+  </si>
+  <si>
+    <t>18 27 Nico HULKENBERG 19.108</t>
+  </si>
+  <si>
+    <t>19 20 Kevin MAGNUSSEN 19.140</t>
+  </si>
+  <si>
+    <t>20 11 Sergio PEREZ 19.475</t>
+  </si>
+  <si>
+    <t>Sector 1 Times (s)</t>
+  </si>
+  <si>
+    <t>All Sector 1</t>
+  </si>
+  <si>
+    <t>44 Lewis HAMILTON 33.929</t>
+  </si>
+  <si>
+    <t>10 Pierre GASLY 34.003</t>
+  </si>
+  <si>
+    <t>63 George RUSSELL 34.101</t>
+  </si>
+  <si>
+    <t>18 Lance STROLL 34.172</t>
+  </si>
+  <si>
+    <t>22 Yuki TSUNODA 34.183</t>
+  </si>
+  <si>
+    <t>4 Lando NORRIS 34.258</t>
+  </si>
+  <si>
+    <t>81 Oscar PIASTRI 34.302</t>
+  </si>
+  <si>
+    <t>21 Nyck DE VRIES 34.307</t>
+  </si>
+  <si>
+    <t>23 Alexander ALBON 34.347</t>
+  </si>
+  <si>
+    <t>77 Valtteri BOTTAS 34.446</t>
+  </si>
+  <si>
+    <t>20 Kevin MAGNUSSEN 34.574</t>
+  </si>
+  <si>
+    <t>2 Logan SARGEANT 34.617</t>
+  </si>
+  <si>
+    <t>27 Nico HULKENBERG 34.707</t>
+  </si>
+  <si>
+    <t>24 ZHOU Guanyu 34.772</t>
+  </si>
+  <si>
+    <t>11 Sergio PEREZ 34.813</t>
+  </si>
+  <si>
+    <t>Sector 2 Times (s)</t>
+  </si>
+  <si>
+    <t>All Sector 2</t>
+  </si>
+  <si>
+    <t>1 Max VERSTAPPEN 18.821</t>
+  </si>
+  <si>
+    <t>31 Esteban OCON 18.922</t>
+  </si>
+  <si>
+    <t>55 Carlos SAINZ 18.935</t>
+  </si>
+  <si>
+    <t>16 Charles LECLERC 18.950</t>
+  </si>
+  <si>
+    <t>44 Lewis HAMILTON 19.039</t>
+  </si>
+  <si>
+    <t>4 Lando NORRIS 19.071</t>
+  </si>
+  <si>
+    <t>10 Pierre GASLY 19.089</t>
+  </si>
+  <si>
+    <t>81 Oscar PIASTRI 19.090</t>
+  </si>
+  <si>
+    <t>22 Yuki TSUNODA 19.105</t>
+  </si>
+  <si>
+    <t>14 Fernando ALONSO 19.109</t>
+  </si>
+  <si>
+    <t>63 George RUSSELL 19.109</t>
+  </si>
+  <si>
+    <t>23 Alexander ALBON 19.161</t>
+  </si>
+  <si>
+    <t>77 Valtteri BOTTAS 19.178</t>
+  </si>
+  <si>
+    <t>21 Nyck DE VRIES 19.221</t>
+  </si>
+  <si>
+    <t>2 Logan SARGEANT 19.423</t>
+  </si>
+  <si>
+    <t>27 Nico HULKENBERG 19.464</t>
+  </si>
+  <si>
+    <t>18 Lance STROLL 19.469</t>
+  </si>
+  <si>
+    <t>24 ZHOU Guanyu 19.497</t>
+  </si>
+  <si>
+    <t>20 Kevin MAGNUSSEN 19.556</t>
+  </si>
+  <si>
+    <t>11 Sergio PEREZ 19.562</t>
+  </si>
+  <si>
+    <t>Sector 3 Times (s)</t>
+  </si>
+  <si>
+    <t>All Sector 3</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +287,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +574,566 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="8.83984375" style="1"/>
+    <col min="8" max="8" width="2.83984375" customWidth="1"/>
+    <col min="9" max="9" width="14.578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.5234375" customWidth="1"/>
+    <col min="11" max="11" width="14.578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.3671875" customWidth="1"/>
+    <col min="13" max="13" width="14.578125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>18.641999999999999</v>
+      </c>
+      <c r="C2" s="2">
+        <v>18.495999999999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>18.651</v>
+      </c>
+      <c r="E2" s="2">
+        <v>18.728000000000002</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>RIGHT(H2,6)</f>
+        <v>18.496</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1" t="str">
+        <f>RIGHT(J2,6)</f>
+        <v>33.844</v>
+      </c>
+      <c r="L2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="1" t="str">
+        <f>RIGHT(L2,6)</f>
+        <v>18.821</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>33.902000000000001</v>
+      </c>
+      <c r="C3" s="2">
+        <v>33.844000000000001</v>
+      </c>
+      <c r="D3" s="2">
+        <v>33.869999999999997</v>
+      </c>
+      <c r="E3" s="2">
+        <v>33.902999999999999</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f t="shared" ref="I3:I21" si="0">RIGHT(H3,6)</f>
+        <v>18.642</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f t="shared" ref="K3:K21" si="1">RIGHT(J3,6)</f>
+        <v>33.856</v>
+      </c>
+      <c r="L3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="1" t="str">
+        <f t="shared" ref="M3:M21" si="2">RIGHT(L3,6)</f>
+        <v>18.922</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>18.821000000000002</v>
+      </c>
+      <c r="C4" s="2">
+        <v>19.109000000000002</v>
+      </c>
+      <c r="D4" s="2">
+        <v>18.95</v>
+      </c>
+      <c r="E4" s="2">
+        <v>18.922000000000001</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18.651</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>33.870</v>
+      </c>
+      <c r="L4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>18.935</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18.665</v>
+      </c>
+      <c r="J5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>33.902</v>
+      </c>
+      <c r="L5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>18.950</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18.728</v>
+      </c>
+      <c r="J6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>33.903</v>
+      </c>
+      <c r="L6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.039</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18.746</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>33.929</v>
+      </c>
+      <c r="L7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.071</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18.757</v>
+      </c>
+      <c r="J8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.003</v>
+      </c>
+      <c r="L8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.089</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18.774</v>
+      </c>
+      <c r="J9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.101</v>
+      </c>
+      <c r="L9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.090</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18.807</v>
+      </c>
+      <c r="J10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.172</v>
+      </c>
+      <c r="L10" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18.839</v>
+      </c>
+      <c r="J11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.183</v>
+      </c>
+      <c r="L11" t="s">
+        <v>58</v>
+      </c>
+      <c r="M11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18.841</v>
+      </c>
+      <c r="J12" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.258</v>
+      </c>
+      <c r="L12" t="s">
+        <v>59</v>
+      </c>
+      <c r="M12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18.853</v>
+      </c>
+      <c r="J13" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.302</v>
+      </c>
+      <c r="L13" t="s">
+        <v>60</v>
+      </c>
+      <c r="M13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18.900</v>
+      </c>
+      <c r="J14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.307</v>
+      </c>
+      <c r="L14" t="s">
+        <v>61</v>
+      </c>
+      <c r="M14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18.914</v>
+      </c>
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.347</v>
+      </c>
+      <c r="L15" t="s">
+        <v>62</v>
+      </c>
+      <c r="M15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18.989</v>
+      </c>
+      <c r="J16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.446</v>
+      </c>
+      <c r="L16" t="s">
+        <v>63</v>
+      </c>
+      <c r="M16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.423</v>
+      </c>
+    </row>
+    <row r="17" spans="8:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>19.070</v>
+      </c>
+      <c r="J17" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.574</v>
+      </c>
+      <c r="L17" t="s">
+        <v>64</v>
+      </c>
+      <c r="M17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.464</v>
+      </c>
+    </row>
+    <row r="18" spans="8:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>19.073</v>
+      </c>
+      <c r="J18" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.617</v>
+      </c>
+      <c r="L18" t="s">
+        <v>65</v>
+      </c>
+      <c r="M18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.469</v>
+      </c>
+    </row>
+    <row r="19" spans="8:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>19.108</v>
+      </c>
+      <c r="J19" t="s">
+        <v>44</v>
+      </c>
+      <c r="K19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.707</v>
+      </c>
+      <c r="L19" t="s">
+        <v>66</v>
+      </c>
+      <c r="M19" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.497</v>
+      </c>
+    </row>
+    <row r="20" spans="8:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>19.140</v>
+      </c>
+      <c r="J20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.772</v>
+      </c>
+      <c r="L20" t="s">
+        <v>67</v>
+      </c>
+      <c r="M20" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.556</v>
+      </c>
+    </row>
+    <row r="21" spans="8:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>19.475</v>
+      </c>
+      <c r="J21" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>34.813</v>
+      </c>
+      <c r="L21" t="s">
+        <v>68</v>
+      </c>
+      <c r="M21" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>19.562</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>